<commit_message>
Major revision of interim report
include data, figures, debugged code for mx variate analyses, etc.
</commit_message>
<xml_diff>
--- a/cost_benefit.xlsx
+++ b/cost_benefit.xlsx
@@ -2763,7 +2763,7 @@
   <dimension ref="A1:BC16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,48 +3104,48 @@
       </c>
       <c r="AN3" s="2"/>
       <c r="AO3" s="2">
-        <f>$AN3/10*1/(POWER(1.08,AO$2-1))</f>
-        <v>0</v>
+        <f>$AM3/10*1/(POWER(1.08,AO$2-1))</f>
+        <v>14855.1</v>
       </c>
       <c r="AP3" s="2">
-        <f t="shared" ref="AP3:AX3" si="3">$AN3/10*1/(POWER(1.08,AP$2-1))</f>
-        <v>0</v>
+        <f t="shared" ref="AP3:AX3" si="3">$AM3/10*1/(POWER(1.08,AP$2-1))</f>
+        <v>13754.722222222221</v>
       </c>
       <c r="AQ3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12735.85390946502</v>
       </c>
       <c r="AR3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11792.457323578721</v>
       </c>
       <c r="AS3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10918.941966276592</v>
       </c>
       <c r="AT3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10110.131450256105</v>
       </c>
       <c r="AU3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9361.2328243112061</v>
       </c>
       <c r="AV3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8667.8081706585253</v>
       </c>
       <c r="AW3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8025.7483061653002</v>
       </c>
       <c r="AX3" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7431.2484316345372</v>
       </c>
       <c r="AY3" s="2">
         <f>SUM(AO3:AX3)</f>
-        <v>0</v>
+        <v>107653.24460456824</v>
       </c>
       <c r="AZ3" s="2"/>
       <c r="BA3" s="3"/>
@@ -3305,48 +3305,48 @@
         <v>127151</v>
       </c>
       <c r="AO4" s="2">
-        <f t="shared" ref="AO4:AX16" si="11">$AN4/10*1/(POWER(1.08,AO$2-1))</f>
-        <v>12715.1</v>
+        <f t="shared" ref="AO4:AX16" si="11">$AM4/10*1/(POWER(1.08,AO$2-1))</f>
+        <v>199972.5</v>
       </c>
       <c r="AP4" s="2">
         <f t="shared" si="11"/>
-        <v>11773.240740740741</v>
+        <v>185159.72222222222</v>
       </c>
       <c r="AQ4" s="2">
         <f t="shared" si="11"/>
-        <v>10901.148834019205</v>
+        <v>171444.18724279833</v>
       </c>
       <c r="AR4" s="2">
         <f t="shared" si="11"/>
-        <v>10093.656327795559</v>
+        <v>158744.61781740587</v>
       </c>
       <c r="AS4" s="2">
         <f t="shared" si="11"/>
-        <v>9345.9780812921836</v>
+        <v>146985.75723833876</v>
       </c>
       <c r="AT4" s="2">
         <f t="shared" si="11"/>
-        <v>8653.6834086038725</v>
+        <v>136097.92336883218</v>
       </c>
       <c r="AU4" s="2">
         <f t="shared" si="11"/>
-        <v>8012.6698227813631</v>
+        <v>126016.59571188163</v>
       </c>
       <c r="AV4" s="2">
         <f t="shared" si="11"/>
-        <v>7419.1387247975581</v>
+        <v>116682.03306655705</v>
       </c>
       <c r="AW4" s="2">
         <f t="shared" si="11"/>
-        <v>6869.572893331072</v>
+        <v>108038.91950607135</v>
       </c>
       <c r="AX4" s="2">
         <f t="shared" si="11"/>
-        <v>6360.7156419732146</v>
+        <v>100036.03657969569</v>
       </c>
       <c r="AY4" s="2">
-        <f t="shared" ref="AY4:AY16" si="12">SUM(AO4:AX4)</f>
-        <v>92144.904475334784</v>
+        <f>SUM(AO4:AX4)</f>
+        <v>1449178.2927538031</v>
       </c>
       <c r="AZ4" s="2">
         <f>W4-AM4</f>
@@ -3358,11 +3358,11 @@
       </c>
       <c r="BB4" s="2">
         <f>AH4-AY4</f>
-        <v>106651015.73224349</v>
+        <v>105293982.34396502</v>
       </c>
       <c r="BC4" s="3">
         <f>BB4/(SUM(AY4,Q4))</f>
-        <v>85.208543838957908</v>
+        <v>40.36292986269784</v>
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.25">
@@ -3383,7 +3383,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" ref="F5:F7" si="13">D5*E5</f>
+        <f t="shared" ref="F5:F7" si="12">D5*E5</f>
         <v>4000000</v>
       </c>
       <c r="G5" s="2">
@@ -3441,7 +3441,7 @@
         <v>0.17</v>
       </c>
       <c r="U5" s="2">
-        <f t="shared" ref="U5:U7" si="14">R5*T5</f>
+        <f t="shared" ref="U5:U7" si="13">R5*T5</f>
         <v>21913.170000000002</v>
       </c>
       <c r="V5" s="2">
@@ -3502,11 +3502,11 @@
         <v>10</v>
       </c>
       <c r="AK5" s="2">
-        <f t="shared" ref="AK5:AK7" si="15">AJ5*AI5</f>
+        <f t="shared" ref="AK5:AK7" si="14">AJ5*AI5</f>
         <v>1750</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" ref="AL5:AL7" si="16">AK5*0.17</f>
+        <f t="shared" ref="AL5:AL7" si="15">AK5*0.17</f>
         <v>297.5</v>
       </c>
       <c r="AM5" s="2">
@@ -3519,47 +3519,47 @@
       </c>
       <c r="AO5" s="2">
         <f t="shared" si="11"/>
-        <v>12715.1</v>
+        <v>199972.5</v>
       </c>
       <c r="AP5" s="2">
         <f t="shared" si="11"/>
-        <v>11773.240740740741</v>
+        <v>185159.72222222222</v>
       </c>
       <c r="AQ5" s="2">
         <f t="shared" si="11"/>
-        <v>10901.148834019205</v>
+        <v>171444.18724279833</v>
       </c>
       <c r="AR5" s="2">
         <f t="shared" si="11"/>
-        <v>10093.656327795559</v>
+        <v>158744.61781740587</v>
       </c>
       <c r="AS5" s="2">
         <f t="shared" si="11"/>
-        <v>9345.9780812921836</v>
+        <v>146985.75723833876</v>
       </c>
       <c r="AT5" s="2">
         <f t="shared" si="11"/>
-        <v>8653.6834086038725</v>
+        <v>136097.92336883218</v>
       </c>
       <c r="AU5" s="2">
         <f t="shared" si="11"/>
-        <v>8012.6698227813631</v>
+        <v>126016.59571188163</v>
       </c>
       <c r="AV5" s="2">
         <f t="shared" si="11"/>
-        <v>7419.1387247975581</v>
+        <v>116682.03306655705</v>
       </c>
       <c r="AW5" s="2">
         <f t="shared" si="11"/>
-        <v>6869.572893331072</v>
+        <v>108038.91950607135</v>
       </c>
       <c r="AX5" s="2">
         <f t="shared" si="11"/>
-        <v>6360.7156419732146</v>
+        <v>100036.03657969569</v>
       </c>
       <c r="AY5" s="2">
-        <f t="shared" si="12"/>
-        <v>92144.904475334784</v>
+        <f t="shared" ref="AY4:AY16" si="16">SUM(AO5:AX5)</f>
+        <v>1449178.2927538031</v>
       </c>
       <c r="AZ5" s="2">
         <f t="shared" ref="AZ5:AZ16" si="17">W5-AM5</f>
@@ -3571,11 +3571,11 @@
       </c>
       <c r="BB5" s="2">
         <f t="shared" ref="BB5:BB16" si="19">AH5-AY5</f>
-        <v>106651015.73224349</v>
+        <v>105293982.34396502</v>
       </c>
       <c r="BC5" s="3">
         <f t="shared" ref="BC5:BC16" si="20">BB5/(SUM(AY5,Q5))</f>
-        <v>35.658501881806608</v>
+        <v>24.217017896653594</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
@@ -3595,7 +3595,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4163060</v>
       </c>
       <c r="G6" s="2">
@@ -3639,7 +3639,7 @@
         <v>208256.64651062919</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" si="5"/>
+        <f>SUM(G6:P6)</f>
         <v>3016922.9186171331</v>
       </c>
       <c r="R6" s="2">
@@ -3653,7 +3653,7 @@
         <v>0.17</v>
       </c>
       <c r="U6" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>57805.440000000002</v>
       </c>
       <c r="V6" s="2">
@@ -3714,11 +3714,11 @@
         <v>10</v>
       </c>
       <c r="AK6" s="2">
+        <f t="shared" si="14"/>
+        <v>1160</v>
+      </c>
+      <c r="AL6" s="2">
         <f t="shared" si="15"/>
-        <v>1160</v>
-      </c>
-      <c r="AL6" s="2">
-        <f t="shared" si="16"/>
         <v>197.20000000000002</v>
       </c>
       <c r="AM6" s="2">
@@ -3731,47 +3731,47 @@
       </c>
       <c r="AO6" s="2">
         <f t="shared" si="11"/>
-        <v>33887.199999999997</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP6" s="2">
         <f t="shared" si="11"/>
-        <v>31377.037037037033</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ6" s="2">
         <f t="shared" si="11"/>
-        <v>29052.812071330583</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR6" s="2">
         <f t="shared" si="11"/>
-        <v>26900.751917898688</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS6" s="2">
         <f t="shared" si="11"/>
-        <v>24908.10362768397</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT6" s="2">
         <f t="shared" si="11"/>
-        <v>23063.058914522193</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU6" s="2">
         <f t="shared" si="11"/>
-        <v>21354.684180113138</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV6" s="2">
         <f t="shared" si="11"/>
-        <v>19772.855722326978</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW6" s="2">
         <f t="shared" si="11"/>
-        <v>18308.199742895351</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX6" s="2">
         <f t="shared" si="11"/>
-        <v>16952.036798977177</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY6" s="2">
-        <f t="shared" si="12"/>
-        <v>245576.74001278513</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ6" s="2">
         <f t="shared" si="17"/>
@@ -3783,11 +3783,11 @@
       </c>
       <c r="BB6" s="2">
         <f t="shared" si="19"/>
-        <v>281335562.2552222</v>
+        <v>280620540.81260961</v>
       </c>
       <c r="BC6" s="3">
         <f t="shared" si="20"/>
-        <v>86.233131553297596</v>
+        <v>70.551615860679775</v>
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.25">
@@ -3807,7 +3807,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>10407650</v>
       </c>
       <c r="G7" s="2">
@@ -3865,7 +3865,7 @@
         <v>0.17</v>
       </c>
       <c r="U7" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>57805.440000000002</v>
       </c>
       <c r="V7" s="2">
@@ -3926,11 +3926,11 @@
         <v>10</v>
       </c>
       <c r="AK7" s="2">
+        <f t="shared" si="14"/>
+        <v>1160</v>
+      </c>
+      <c r="AL7" s="2">
         <f t="shared" si="15"/>
-        <v>1160</v>
-      </c>
-      <c r="AL7" s="2">
-        <f t="shared" si="16"/>
         <v>197.20000000000002</v>
       </c>
       <c r="AM7" s="2">
@@ -3943,47 +3943,47 @@
       </c>
       <c r="AO7" s="2">
         <f t="shared" si="11"/>
-        <v>33887.199999999997</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP7" s="2">
         <f t="shared" si="11"/>
-        <v>31377.037037037033</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ7" s="2">
         <f t="shared" si="11"/>
-        <v>29052.812071330583</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR7" s="2">
         <f t="shared" si="11"/>
-        <v>26900.751917898688</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS7" s="2">
         <f t="shared" si="11"/>
-        <v>24908.10362768397</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT7" s="2">
         <f t="shared" si="11"/>
-        <v>23063.058914522193</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU7" s="2">
         <f t="shared" si="11"/>
-        <v>21354.684180113138</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV7" s="2">
         <f t="shared" si="11"/>
-        <v>19772.855722326978</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW7" s="2">
         <f t="shared" si="11"/>
-        <v>18308.199742895351</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX7" s="2">
         <f t="shared" si="11"/>
-        <v>16952.036798977177</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY7" s="2">
-        <f t="shared" si="12"/>
-        <v>245576.74001278513</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ7" s="2">
         <f t="shared" si="17"/>
@@ -3994,12 +3994,12 @@
         <v>33.002900185133065</v>
       </c>
       <c r="BB7" s="2">
-        <f t="shared" si="19"/>
-        <v>281335562.2552222</v>
+        <f>AH7-AY7</f>
+        <v>280620540.81260961</v>
       </c>
       <c r="BC7" s="3">
         <f t="shared" si="20"/>
-        <v>36.124775476195936</v>
+        <v>33.002900185133079</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
@@ -4156,47 +4156,47 @@
       </c>
       <c r="AO8" s="2">
         <f t="shared" si="11"/>
-        <v>38091.4</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP8" s="2">
         <f t="shared" si="11"/>
-        <v>35269.81481481481</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ8" s="2">
         <f t="shared" si="11"/>
-        <v>32657.235939643346</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR8" s="2">
         <f t="shared" si="11"/>
-        <v>30238.181425595689</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS8" s="2">
         <f t="shared" si="11"/>
-        <v>27998.316134810819</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT8" s="2">
         <f t="shared" si="11"/>
-        <v>25924.366791491502</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU8" s="2">
         <f t="shared" si="11"/>
-        <v>24004.043325455092</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV8" s="2">
         <f t="shared" si="11"/>
-        <v>22225.966042088046</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW8" s="2">
         <f t="shared" si="11"/>
-        <v>20579.598187118561</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX8" s="2">
         <f t="shared" si="11"/>
-        <v>19055.18350659126</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY8" s="2">
-        <f t="shared" si="12"/>
-        <v>276044.10616760916</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ8" s="2">
         <f t="shared" si="17"/>
@@ -4208,11 +4208,11 @@
       </c>
       <c r="BB8" s="2">
         <f t="shared" si="19"/>
-        <v>316120154.19418472</v>
+        <v>315435600.11772698</v>
       </c>
       <c r="BC8" s="3">
         <f t="shared" si="20"/>
-        <v>80.302703467918874</v>
+        <v>68.258954997779441</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.25">
@@ -4369,47 +4369,47 @@
       </c>
       <c r="AO9" s="2">
         <f t="shared" si="11"/>
-        <v>38091.4</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP9" s="2">
         <f t="shared" si="11"/>
-        <v>35269.81481481481</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ9" s="2">
         <f t="shared" si="11"/>
-        <v>32657.235939643346</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR9" s="2">
         <f t="shared" si="11"/>
-        <v>30238.181425595689</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS9" s="2">
         <f t="shared" si="11"/>
-        <v>27998.316134810819</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT9" s="2">
         <f t="shared" si="11"/>
-        <v>25924.366791491502</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU9" s="2">
         <f t="shared" si="11"/>
-        <v>24004.043325455092</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV9" s="2">
         <f t="shared" si="11"/>
-        <v>22225.966042088046</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW9" s="2">
         <f t="shared" si="11"/>
-        <v>20579.598187118561</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX9" s="2">
         <f t="shared" si="11"/>
-        <v>19055.18350659126</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY9" s="2">
-        <f t="shared" si="12"/>
-        <v>276044.10616760916</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ9" s="2">
         <f t="shared" si="17"/>
@@ -4421,11 +4421,11 @@
       </c>
       <c r="BB9" s="2">
         <f t="shared" si="19"/>
-        <v>316120154.19418472</v>
+        <v>315435600.11772698</v>
       </c>
       <c r="BC9" s="3">
         <f t="shared" si="20"/>
-        <v>33.53188200074964</v>
+        <v>31.194171346110277</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
@@ -4576,47 +4576,47 @@
       <c r="AN10" s="2"/>
       <c r="AO10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>14855.1</v>
       </c>
       <c r="AP10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>13754.722222222221</v>
       </c>
       <c r="AQ10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>12735.85390946502</v>
       </c>
       <c r="AR10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>11792.457323578721</v>
       </c>
       <c r="AS10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10918.941966276592</v>
       </c>
       <c r="AT10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>10110.131450256105</v>
       </c>
       <c r="AU10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>9361.2328243112061</v>
       </c>
       <c r="AV10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8667.8081706585253</v>
       </c>
       <c r="AW10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8025.7483061653002</v>
       </c>
       <c r="AX10" s="2">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>7431.2484316345372</v>
       </c>
       <c r="AY10" s="2">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>107653.24460456824</v>
       </c>
       <c r="AZ10" s="2"/>
       <c r="BA10" s="3"/>
@@ -4685,7 +4685,7 @@
         <v>80039.834741033439</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" si="5"/>
+        <f>SUM(G11:P11)</f>
         <v>1159502.0657370812</v>
       </c>
       <c r="R11" s="2">
@@ -4777,47 +4777,47 @@
       </c>
       <c r="AO11" s="2">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>199972.5</v>
       </c>
       <c r="AP11" s="2">
         <f t="shared" si="11"/>
-        <v>41.666666666666664</v>
+        <v>185159.72222222222</v>
       </c>
       <c r="AQ11" s="2">
         <f t="shared" si="11"/>
-        <v>38.580246913580247</v>
+        <v>171444.18724279833</v>
       </c>
       <c r="AR11" s="2">
         <f t="shared" si="11"/>
-        <v>35.72245084590763</v>
+        <v>158744.61781740587</v>
       </c>
       <c r="AS11" s="2">
         <f t="shared" si="11"/>
-        <v>33.076343375840395</v>
+        <v>146985.75723833876</v>
       </c>
       <c r="AT11" s="2">
         <f t="shared" si="11"/>
-        <v>30.626243866518884</v>
+        <v>136097.92336883218</v>
       </c>
       <c r="AU11" s="2">
         <f t="shared" si="11"/>
-        <v>28.357633209739706</v>
+        <v>126016.59571188163</v>
       </c>
       <c r="AV11" s="2">
         <f t="shared" si="11"/>
-        <v>26.257067786796021</v>
+        <v>116682.03306655705</v>
       </c>
       <c r="AW11" s="2">
         <f t="shared" si="11"/>
-        <v>24.312099802588911</v>
+        <v>108038.91950607135</v>
       </c>
       <c r="AX11" s="2">
         <f t="shared" si="11"/>
-        <v>22.511203520915654</v>
+        <v>100036.03657969569</v>
       </c>
       <c r="AY11" s="2">
-        <f t="shared" si="12"/>
-        <v>326.10995598855413</v>
+        <f t="shared" si="16"/>
+        <v>1449178.2927538031</v>
       </c>
       <c r="AZ11" s="2">
         <f t="shared" si="17"/>
@@ -4829,11 +4829,11 @@
       </c>
       <c r="BB11" s="2">
         <f t="shared" si="19"/>
-        <v>1821498.029505935</v>
+        <v>372645.84670812055</v>
       </c>
       <c r="BC11" s="3">
         <f t="shared" si="20"/>
-        <v>1.5704895498141147</v>
+        <v>0.14284841203147453</v>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
@@ -4990,47 +4990,47 @@
       </c>
       <c r="AO12" s="2">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>199972.5</v>
       </c>
       <c r="AP12" s="2">
         <f t="shared" si="11"/>
-        <v>41.666666666666664</v>
+        <v>185159.72222222222</v>
       </c>
       <c r="AQ12" s="2">
         <f t="shared" si="11"/>
-        <v>38.580246913580247</v>
+        <v>171444.18724279833</v>
       </c>
       <c r="AR12" s="2">
         <f t="shared" si="11"/>
-        <v>35.72245084590763</v>
+        <v>158744.61781740587</v>
       </c>
       <c r="AS12" s="2">
         <f t="shared" si="11"/>
-        <v>33.076343375840395</v>
+        <v>146985.75723833876</v>
       </c>
       <c r="AT12" s="2">
         <f t="shared" si="11"/>
-        <v>30.626243866518884</v>
+        <v>136097.92336883218</v>
       </c>
       <c r="AU12" s="2">
         <f t="shared" si="11"/>
-        <v>28.357633209739706</v>
+        <v>126016.59571188163</v>
       </c>
       <c r="AV12" s="2">
         <f t="shared" si="11"/>
-        <v>26.257067786796021</v>
+        <v>116682.03306655705</v>
       </c>
       <c r="AW12" s="2">
         <f t="shared" si="11"/>
-        <v>24.312099802588911</v>
+        <v>108038.91950607135</v>
       </c>
       <c r="AX12" s="2">
         <f t="shared" si="11"/>
-        <v>22.511203520915654</v>
+        <v>100036.03657969569</v>
       </c>
       <c r="AY12" s="2">
-        <f t="shared" si="12"/>
-        <v>326.10995598855413</v>
+        <f t="shared" si="16"/>
+        <v>1449178.2927538031</v>
       </c>
       <c r="AZ12" s="2">
         <f t="shared" si="17"/>
@@ -5042,11 +5042,11 @@
       </c>
       <c r="BB12" s="2">
         <f t="shared" si="19"/>
-        <v>1821498.029505935</v>
+        <v>372645.84670812055</v>
       </c>
       <c r="BC12" s="3">
         <f t="shared" si="20"/>
-        <v>0.62830181604569491</v>
+        <v>8.570642821129297E-2</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
@@ -5202,47 +5202,47 @@
       </c>
       <c r="AO13" s="2">
         <f t="shared" si="11"/>
-        <v>104</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP13" s="2">
         <f t="shared" si="11"/>
-        <v>96.296296296296291</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ13" s="2">
         <f t="shared" si="11"/>
-        <v>89.163237311385458</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR13" s="2">
         <f t="shared" si="11"/>
-        <v>82.55855306609763</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS13" s="2">
         <f t="shared" si="11"/>
-        <v>76.443104690831134</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT13" s="2">
         <f t="shared" si="11"/>
-        <v>70.78065249151031</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU13" s="2">
         <f t="shared" si="11"/>
-        <v>65.53764119584288</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV13" s="2">
         <f t="shared" si="11"/>
-        <v>60.683001107261916</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW13" s="2">
         <f t="shared" si="11"/>
-        <v>56.187963988205482</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX13" s="2">
         <f t="shared" si="11"/>
-        <v>52.025892581671734</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY13" s="2">
-        <f t="shared" si="12"/>
-        <v>753.676342729103</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ13" s="2">
         <f t="shared" si="17"/>
@@ -5254,11 +5254,11 @@
       </c>
       <c r="BB13" s="2">
         <f t="shared" si="19"/>
-        <v>1821070.4631191946</v>
+        <v>861225.95683654549</v>
       </c>
       <c r="BC13" s="3">
         <f t="shared" si="20"/>
-        <v>0.60346773612545335</v>
+        <v>0.21652329049053012</v>
       </c>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
@@ -5414,47 +5414,47 @@
       </c>
       <c r="AO14" s="2">
         <f t="shared" si="11"/>
-        <v>104</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP14" s="2">
         <f t="shared" si="11"/>
-        <v>96.296296296296291</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ14" s="2">
         <f t="shared" si="11"/>
-        <v>89.163237311385458</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR14" s="2">
         <f t="shared" si="11"/>
-        <v>82.55855306609763</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS14" s="2">
         <f t="shared" si="11"/>
-        <v>76.443104690831134</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT14" s="2">
         <f t="shared" si="11"/>
-        <v>70.78065249151031</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU14" s="2">
         <f t="shared" si="11"/>
-        <v>65.53764119584288</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV14" s="2">
         <f t="shared" si="11"/>
-        <v>60.683001107261916</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW14" s="2">
         <f t="shared" si="11"/>
-        <v>56.187963988205482</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX14" s="2">
         <f t="shared" si="11"/>
-        <v>52.025892581671734</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY14" s="2">
-        <f t="shared" si="12"/>
-        <v>753.676342729103</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ14" s="2">
         <f t="shared" si="17"/>
@@ -5466,11 +5466,11 @@
       </c>
       <c r="BB14" s="2">
         <f t="shared" si="19"/>
-        <v>1821070.4631191946</v>
+        <v>861225.95683654549</v>
       </c>
       <c r="BC14" s="3">
         <f t="shared" si="20"/>
-        <v>0.24142327228498495</v>
+        <v>0.1012860790874973</v>
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
@@ -5627,47 +5627,47 @@
       </c>
       <c r="AO15" s="2">
         <f t="shared" si="11"/>
-        <v>104</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP15" s="2">
         <f t="shared" si="11"/>
-        <v>96.296296296296291</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ15" s="2">
         <f t="shared" si="11"/>
-        <v>89.163237311385458</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR15" s="2">
         <f t="shared" si="11"/>
-        <v>82.55855306609763</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS15" s="2">
         <f t="shared" si="11"/>
-        <v>76.443104690831134</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT15" s="2">
         <f t="shared" si="11"/>
-        <v>70.78065249151031</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU15" s="2">
         <f t="shared" si="11"/>
-        <v>65.53764119584288</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV15" s="2">
         <f t="shared" si="11"/>
-        <v>60.683001107261916</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW15" s="2">
         <f t="shared" si="11"/>
-        <v>56.187963988205482</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX15" s="2">
         <f t="shared" si="11"/>
-        <v>52.025892581671734</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY15" s="2">
-        <f t="shared" si="12"/>
-        <v>753.676342729103</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ15" s="2">
         <f t="shared" si="17"/>
@@ -5679,11 +5679,11 @@
       </c>
       <c r="BB15" s="2">
         <f t="shared" si="19"/>
-        <v>1821070.4631191946</v>
+        <v>861225.95683654549</v>
       </c>
       <c r="BC15" s="3">
         <f t="shared" si="20"/>
-        <v>0.49738136992157961</v>
+        <v>0.18636572349057945</v>
       </c>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
@@ -5840,47 +5840,47 @@
       </c>
       <c r="AO16" s="2">
         <f t="shared" si="11"/>
-        <v>104</v>
+        <v>132553.20000000001</v>
       </c>
       <c r="AP16" s="2">
         <f t="shared" si="11"/>
-        <v>96.296296296296291</v>
+        <v>122734.44444444445</v>
       </c>
       <c r="AQ16" s="2">
         <f t="shared" si="11"/>
-        <v>89.163237311385458</v>
+        <v>113643.00411522634</v>
       </c>
       <c r="AR16" s="2">
         <f t="shared" si="11"/>
-        <v>82.55855306609763</v>
+        <v>105225.00381039476</v>
       </c>
       <c r="AS16" s="2">
         <f t="shared" si="11"/>
-        <v>76.443104690831134</v>
+        <v>97430.559083698841</v>
       </c>
       <c r="AT16" s="2">
         <f t="shared" si="11"/>
-        <v>70.78065249151031</v>
+        <v>90213.480633054482</v>
       </c>
       <c r="AU16" s="2">
         <f t="shared" si="11"/>
-        <v>65.53764119584288</v>
+        <v>83531.00058616155</v>
       </c>
       <c r="AV16" s="2">
         <f t="shared" si="11"/>
-        <v>60.683001107261916</v>
+        <v>77343.519061260682</v>
       </c>
       <c r="AW16" s="2">
         <f t="shared" si="11"/>
-        <v>56.187963988205482</v>
+        <v>71614.369501167297</v>
       </c>
       <c r="AX16" s="2">
         <f t="shared" si="11"/>
-        <v>52.025892581671734</v>
+        <v>66309.601389969714</v>
       </c>
       <c r="AY16" s="2">
-        <f t="shared" si="12"/>
-        <v>753.676342729103</v>
+        <f t="shared" si="16"/>
+        <v>960598.18262537813</v>
       </c>
       <c r="AZ16" s="2">
         <f t="shared" si="17"/>
@@ -5892,11 +5892,11 @@
       </c>
       <c r="BB16" s="2">
         <f t="shared" si="19"/>
-        <v>1821070.4631191946</v>
+        <v>861225.95683654549</v>
       </c>
       <c r="BC16" s="3">
         <f t="shared" si="20"/>
-        <v>0.19897712345069993</v>
+        <v>8.5168668518234222E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Figures and cost benefit changes
Large changes to sweave code, especially relating to figures, and
altered c/b ratio analyses after going through with Tim
</commit_message>
<xml_diff>
--- a/cost_benefit.xlsx
+++ b/cost_benefit.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="44">
   <si>
     <t>0.92-1.19</t>
   </si>
@@ -142,7 +142,13 @@
     <t>year</t>
   </si>
   <si>
-    <t>Revised costs</t>
+    <t>Revised vaccine discounted costs</t>
+  </si>
+  <si>
+    <t>revised discounted case costs</t>
+  </si>
+  <si>
+    <t>Revised discounted case costs</t>
   </si>
 </sst>
 </file>
@@ -2762,8 +2768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2891,7 +2897,7 @@
         <v>10</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>16</v>
@@ -2942,7 +2948,7 @@
         <v>10</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AZ2" s="1" t="s">
         <v>2</v>
@@ -3558,7 +3564,7 @@
         <v>100036.03657969569</v>
       </c>
       <c r="AY5" s="2">
-        <f t="shared" ref="AY4:AY16" si="16">SUM(AO5:AX5)</f>
+        <f t="shared" ref="AY5:AY16" si="16">SUM(AO5:AX5)</f>
         <v>1449178.2927538031</v>
       </c>
       <c r="AZ5" s="2">

</xml_diff>